<commit_message>
atualização e organização de códigos no jupyter notebook
</commit_message>
<xml_diff>
--- a/base de dados e códigos/comparacao_algoritmos_machine_learning_com_odds.xlsx
+++ b/base de dados e códigos/comparacao_algoritmos_machine_learning_com_odds.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\André\Documents\Eng. Computação\2020.1\TCC\base de dados e códigos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{260C7CD7-FB32-42E8-A7EE-2327705C42DA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BD3FC11-7A9C-438F-ABA7-44060CCA2090}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,9 +25,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
-    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="ExcelA1"/>
-    </ext>
   </extLst>
 </workbook>
 </file>
@@ -146,9 +143,6 @@
     <t>Árvore</t>
   </si>
   <si>
-    <t>Regras</t>
-  </si>
-  <si>
     <t>kNN</t>
   </si>
   <si>
@@ -165,6 +159,9 @@
   </si>
   <si>
     <t>Random Forest</t>
+  </si>
+  <si>
+    <t>ODDS</t>
   </si>
 </sst>
 </file>
@@ -247,7 +244,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -274,6 +271,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -659,8 +662,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R37"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A21" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H36" sqref="H36"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -705,22 +708,22 @@
         <v>36</v>
       </c>
       <c r="D5" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="F5" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="G5" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="H5" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="H5" s="2" t="s">
-        <v>40</v>
-      </c>
       <c r="I5" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J5" s="3"/>
       <c r="K5" s="2" t="s">
@@ -730,22 +733,22 @@
         <v>36</v>
       </c>
       <c r="M5" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="N5" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="N5" s="2" t="s">
+      <c r="O5" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="O5" s="2" t="s">
+      <c r="P5" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="P5" s="2" t="s">
+      <c r="Q5" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="Q5" s="2" t="s">
-        <v>40</v>
-      </c>
       <c r="R5" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
@@ -761,7 +764,9 @@
       <c r="D6" s="4">
         <v>0.63478999651446499</v>
       </c>
-      <c r="E6" s="4"/>
+      <c r="E6" s="12">
+        <v>0.55419135587312596</v>
+      </c>
       <c r="F6" s="4">
         <v>0.56744945974206995</v>
       </c>
@@ -774,19 +779,19 @@
       </c>
       <c r="K6" s="6">
         <f t="shared" ref="K6:K35" si="0">_xlfn.RANK.AVG(B6,B6:I6)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="L6" s="6">
         <f t="shared" ref="L6:L35" si="1">_xlfn.RANK.AVG(C6,B6:I6)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="M6" s="6">
         <f>_xlfn.RANK.AVG(D6,B6:I6)</f>
         <v>1</v>
       </c>
-      <c r="N6" s="6" t="e">
+      <c r="N6" s="6">
         <f t="shared" ref="N6:N35" si="2">_xlfn.RANK.AVG(E6,B6:I6)</f>
-        <v>#N/A</v>
+        <v>5</v>
       </c>
       <c r="O6" s="6">
         <f t="shared" ref="O6:O35" si="3">_xlfn.RANK.AVG(F6,B6:I6)</f>
@@ -818,7 +823,9 @@
       <c r="D7" s="4">
         <v>0.638667654234925</v>
       </c>
-      <c r="E7" s="4"/>
+      <c r="E7" s="12">
+        <v>0.55415214360404297</v>
+      </c>
       <c r="F7" s="4">
         <v>0.55547664691530096</v>
       </c>
@@ -831,19 +838,19 @@
       </c>
       <c r="K7" s="6">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="L7" s="6">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="M7" s="6">
         <f t="shared" ref="M7:M35" si="7">_xlfn.RANK.AVG(D7,B7:I7)</f>
         <v>1</v>
       </c>
-      <c r="N7" s="6" t="e">
-        <f t="shared" si="2"/>
-        <v>#N/A</v>
+      <c r="N7" s="6">
+        <f t="shared" si="2"/>
+        <v>5</v>
       </c>
       <c r="O7" s="6">
         <f t="shared" si="3"/>
@@ -875,7 +882,9 @@
       <c r="D8" s="4">
         <v>0.64071540606483102</v>
       </c>
-      <c r="E8" s="4"/>
+      <c r="E8" s="12">
+        <v>0.55404757755315404</v>
+      </c>
       <c r="F8" s="4">
         <v>0.55212181944928496</v>
       </c>
@@ -888,23 +897,23 @@
       </c>
       <c r="K8" s="6">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="L8" s="6">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="M8" s="6">
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
-      <c r="N8" s="6" t="e">
-        <f t="shared" si="2"/>
-        <v>#N/A</v>
+      <c r="N8" s="6">
+        <f t="shared" si="2"/>
+        <v>4</v>
       </c>
       <c r="O8" s="6">
         <f t="shared" si="3"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="P8" s="6" t="e">
         <f t="shared" si="4"/>
@@ -932,7 +941,9 @@
       <c r="D9" s="4">
         <v>0.62940920181247795</v>
       </c>
-      <c r="E9" s="4"/>
+      <c r="E9" s="12">
+        <v>0.55420442662948699</v>
+      </c>
       <c r="F9" s="4">
         <v>0.55419135587312596</v>
       </c>
@@ -949,19 +960,19 @@
       </c>
       <c r="L9" s="6">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="M9" s="6">
         <f t="shared" si="7"/>
         <v>2</v>
       </c>
-      <c r="N9" s="6" t="e">
-        <f t="shared" si="2"/>
-        <v>#N/A</v>
+      <c r="N9" s="6">
+        <f t="shared" si="2"/>
+        <v>5</v>
       </c>
       <c r="O9" s="6">
         <f t="shared" si="3"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="P9" s="6" t="e">
         <f t="shared" si="4"/>
@@ -989,7 +1000,9 @@
       <c r="D10" s="4">
         <v>0.63205385151620697</v>
       </c>
-      <c r="E10" s="4"/>
+      <c r="E10" s="12">
+        <v>0.55421314046706105</v>
+      </c>
       <c r="F10" s="4">
         <v>0.55945887068665001</v>
       </c>
@@ -1002,19 +1015,19 @@
       </c>
       <c r="K10" s="6">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="L10" s="6">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="M10" s="6">
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
-      <c r="N10" s="6" t="e">
-        <f t="shared" si="2"/>
-        <v>#N/A</v>
+      <c r="N10" s="6">
+        <f t="shared" si="2"/>
+        <v>5</v>
       </c>
       <c r="O10" s="6">
         <f t="shared" si="3"/>
@@ -1046,7 +1059,9 @@
       <c r="D11" s="4">
         <v>0.63998780062739602</v>
       </c>
-      <c r="E11" s="4"/>
+      <c r="E11" s="12">
+        <v>0.55420878354827396</v>
+      </c>
       <c r="F11" s="4">
         <v>0.55544179156500495</v>
       </c>
@@ -1063,15 +1078,15 @@
       </c>
       <c r="L11" s="6">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="M11" s="6">
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
-      <c r="N11" s="6" t="e">
-        <f t="shared" si="2"/>
-        <v>#N/A</v>
+      <c r="N11" s="6">
+        <f t="shared" si="2"/>
+        <v>6</v>
       </c>
       <c r="O11" s="6">
         <f t="shared" si="3"/>
@@ -1103,7 +1118,9 @@
       <c r="D12" s="4">
         <v>0.64466713140467002</v>
       </c>
-      <c r="E12" s="4"/>
+      <c r="E12" s="12">
+        <v>0.55418264203555201</v>
+      </c>
       <c r="F12" s="4">
         <v>0.56010805158591803</v>
       </c>
@@ -1116,19 +1133,19 @@
       </c>
       <c r="K12" s="6">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="L12" s="6">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="M12" s="6">
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
-      <c r="N12" s="6" t="e">
-        <f t="shared" si="2"/>
-        <v>#N/A</v>
+      <c r="N12" s="6">
+        <f t="shared" si="2"/>
+        <v>5</v>
       </c>
       <c r="O12" s="6">
         <f t="shared" si="3"/>
@@ -1160,7 +1177,9 @@
       <c r="D13" s="4">
         <v>0.64535116765423495</v>
       </c>
-      <c r="E13" s="4"/>
+      <c r="E13" s="12">
+        <v>0.55407371906587599</v>
+      </c>
       <c r="F13" s="4">
         <v>0.56471767166260001</v>
       </c>
@@ -1173,19 +1192,19 @@
       </c>
       <c r="K13" s="6">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="L13" s="6">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="M13" s="6">
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
-      <c r="N13" s="6" t="e">
-        <f t="shared" si="2"/>
-        <v>#N/A</v>
+      <c r="N13" s="6">
+        <f t="shared" si="2"/>
+        <v>5</v>
       </c>
       <c r="O13" s="6">
         <f t="shared" si="3"/>
@@ -1217,7 +1236,9 @@
       <c r="D14" s="4">
         <v>0.64465841756709596</v>
       </c>
-      <c r="E14" s="4"/>
+      <c r="E14" s="12">
+        <v>0.55416957127919098</v>
+      </c>
       <c r="F14" s="4">
         <v>0.55087138375740596</v>
       </c>
@@ -1230,23 +1251,23 @@
       </c>
       <c r="K14" s="6">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="L14" s="6">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="M14" s="6">
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
-      <c r="N14" s="6" t="e">
-        <f t="shared" si="2"/>
-        <v>#N/A</v>
+      <c r="N14" s="6">
+        <f t="shared" si="2"/>
+        <v>4</v>
       </c>
       <c r="O14" s="6">
         <f t="shared" si="3"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="P14" s="6" t="e">
         <f t="shared" si="4"/>
@@ -1274,7 +1295,9 @@
       <c r="D15" s="4">
         <v>0.63670704078075901</v>
       </c>
-      <c r="E15" s="4"/>
+      <c r="E15" s="12">
+        <v>0.554165214360404</v>
+      </c>
       <c r="F15" s="4">
         <v>0.55810386894388198</v>
       </c>
@@ -1287,19 +1310,19 @@
       </c>
       <c r="K15" s="6">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="L15" s="6">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="M15" s="6">
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
-      <c r="N15" s="6" t="e">
-        <f t="shared" si="2"/>
-        <v>#N/A</v>
+      <c r="N15" s="6">
+        <f t="shared" si="2"/>
+        <v>5</v>
       </c>
       <c r="O15" s="6">
         <f t="shared" si="3"/>
@@ -1331,7 +1354,9 @@
       <c r="D16" s="4">
         <v>0.65450505402579195</v>
       </c>
-      <c r="E16" s="4"/>
+      <c r="E16" s="12">
+        <v>0.55414342976646902</v>
+      </c>
       <c r="F16" s="4">
         <v>0.55813872429417899</v>
       </c>
@@ -1348,15 +1373,15 @@
       </c>
       <c r="L16" s="6">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="M16" s="6">
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
-      <c r="N16" s="6" t="e">
-        <f t="shared" si="2"/>
-        <v>#N/A</v>
+      <c r="N16" s="6">
+        <f t="shared" si="2"/>
+        <v>6</v>
       </c>
       <c r="O16" s="6">
         <f t="shared" si="3"/>
@@ -1388,7 +1413,9 @@
       <c r="D17" s="4">
         <v>0.641334088532589</v>
       </c>
-      <c r="E17" s="4"/>
+      <c r="E17" s="12">
+        <v>0.55415214360404297</v>
+      </c>
       <c r="F17" s="4">
         <v>0.56141948414081499</v>
       </c>
@@ -1401,19 +1428,19 @@
       </c>
       <c r="K17" s="6">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="L17" s="6">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="M17" s="6">
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
-      <c r="N17" s="6" t="e">
-        <f t="shared" si="2"/>
-        <v>#N/A</v>
+      <c r="N17" s="6">
+        <f t="shared" si="2"/>
+        <v>5</v>
       </c>
       <c r="O17" s="6">
         <f t="shared" si="3"/>
@@ -1445,7 +1472,9 @@
       <c r="D18" s="4">
         <v>0.63408853258975195</v>
       </c>
-      <c r="E18" s="4"/>
+      <c r="E18" s="12">
+        <v>0.55418264203555201</v>
+      </c>
       <c r="F18" s="4">
         <v>0.55555942837225503</v>
       </c>
@@ -1458,19 +1487,19 @@
       </c>
       <c r="K18" s="6">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="L18" s="6">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="M18" s="6">
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
-      <c r="N18" s="6" t="e">
-        <f t="shared" si="2"/>
-        <v>#N/A</v>
+      <c r="N18" s="6">
+        <f t="shared" si="2"/>
+        <v>5</v>
       </c>
       <c r="O18" s="6">
         <f t="shared" si="3"/>
@@ -1502,7 +1531,9 @@
       <c r="D19" s="4">
         <v>0.63934297664691497</v>
       </c>
-      <c r="E19" s="4"/>
+      <c r="E19" s="12">
+        <v>0.55415650052283005</v>
+      </c>
       <c r="F19" s="4">
         <v>0.56012547926106604</v>
       </c>
@@ -1515,19 +1546,19 @@
       </c>
       <c r="K19" s="6">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="L19" s="6">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="M19" s="6">
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
-      <c r="N19" s="6" t="e">
-        <f t="shared" si="2"/>
-        <v>#N/A</v>
+      <c r="N19" s="6">
+        <f t="shared" si="2"/>
+        <v>5</v>
       </c>
       <c r="O19" s="6">
         <f t="shared" si="3"/>
@@ -1559,7 +1590,9 @@
       <c r="D20" s="4">
         <v>0.64132973161380202</v>
       </c>
-      <c r="E20" s="4"/>
+      <c r="E20" s="12">
+        <v>0.55416085744161703</v>
+      </c>
       <c r="F20" s="4">
         <v>0.56209916347159194</v>
       </c>
@@ -1572,19 +1605,19 @@
       </c>
       <c r="K20" s="6">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="L20" s="6">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="M20" s="6">
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
-      <c r="N20" s="6" t="e">
-        <f t="shared" si="2"/>
-        <v>#N/A</v>
+      <c r="N20" s="6">
+        <f t="shared" si="2"/>
+        <v>5</v>
       </c>
       <c r="O20" s="6">
         <f t="shared" si="3"/>
@@ -1616,7 +1649,9 @@
       <c r="D21" s="4">
         <v>0.64856221680027804</v>
       </c>
-      <c r="E21" s="4"/>
+      <c r="E21" s="12">
+        <v>0.55419135587312596</v>
+      </c>
       <c r="F21" s="4">
         <v>0.56478738236319204</v>
       </c>
@@ -1629,19 +1664,19 @@
       </c>
       <c r="K21" s="6">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="L21" s="6">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="M21" s="6">
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
-      <c r="N21" s="6" t="e">
-        <f t="shared" si="2"/>
-        <v>#N/A</v>
+      <c r="N21" s="6">
+        <f t="shared" si="2"/>
+        <v>5</v>
       </c>
       <c r="O21" s="6">
         <f t="shared" si="3"/>
@@ -1673,7 +1708,9 @@
       <c r="D22" s="4">
         <v>0.63273353084698503</v>
       </c>
-      <c r="E22" s="4"/>
+      <c r="E22" s="12">
+        <v>0.554221854304635</v>
+      </c>
       <c r="F22" s="4">
         <v>0.56671749738584798</v>
       </c>
@@ -1686,19 +1723,19 @@
       </c>
       <c r="K22" s="6">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="L22" s="6">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="M22" s="6">
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
-      <c r="N22" s="6" t="e">
-        <f t="shared" si="2"/>
-        <v>#N/A</v>
+      <c r="N22" s="6">
+        <f t="shared" si="2"/>
+        <v>5</v>
       </c>
       <c r="O22" s="6">
         <f t="shared" si="3"/>
@@ -1730,7 +1767,9 @@
       <c r="D23" s="4">
         <v>0.64199634018821805</v>
       </c>
-      <c r="E23" s="4"/>
+      <c r="E23" s="12">
+        <v>0.55418699895433898</v>
+      </c>
       <c r="F23" s="4">
         <v>0.55417828511676503</v>
       </c>
@@ -1747,19 +1786,19 @@
       </c>
       <c r="L23" s="6">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="M23" s="6">
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
-      <c r="N23" s="6" t="e">
-        <f t="shared" si="2"/>
-        <v>#N/A</v>
+      <c r="N23" s="6">
+        <f t="shared" si="2"/>
+        <v>5</v>
       </c>
       <c r="O23" s="6">
         <f t="shared" si="3"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="P23" s="6" t="e">
         <f t="shared" si="4"/>
@@ -1787,7 +1826,9 @@
       <c r="D24" s="4">
         <v>0.64072411990240496</v>
       </c>
-      <c r="E24" s="4"/>
+      <c r="E24" s="12">
+        <v>0.55418699895433898</v>
+      </c>
       <c r="F24" s="4">
         <v>0.55939351690484496</v>
       </c>
@@ -1800,19 +1841,19 @@
       </c>
       <c r="K24" s="6">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="L24" s="6">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="M24" s="6">
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
-      <c r="N24" s="6" t="e">
-        <f t="shared" si="2"/>
-        <v>#N/A</v>
+      <c r="N24" s="6">
+        <f t="shared" si="2"/>
+        <v>5</v>
       </c>
       <c r="O24" s="6">
         <f t="shared" si="3"/>
@@ -1844,7 +1885,9 @@
       <c r="D25" s="4">
         <v>0.63682467758800898</v>
       </c>
-      <c r="E25" s="4"/>
+      <c r="E25" s="12">
+        <v>0.55418699895433898</v>
+      </c>
       <c r="F25" s="4">
         <v>0.54887591495294497</v>
       </c>
@@ -1857,23 +1900,23 @@
       </c>
       <c r="K25" s="6">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="L25" s="6">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="M25" s="6">
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
-      <c r="N25" s="6" t="e">
-        <f t="shared" si="2"/>
-        <v>#N/A</v>
+      <c r="N25" s="6">
+        <f t="shared" si="2"/>
+        <v>4</v>
       </c>
       <c r="O25" s="6">
         <f t="shared" si="3"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="P25" s="6" t="e">
         <f t="shared" si="4"/>
@@ -1901,7 +1944,9 @@
       <c r="D26" s="4">
         <v>0.63805768560473997</v>
       </c>
-      <c r="E26" s="4"/>
+      <c r="E26" s="12">
+        <v>0.55411293133495998</v>
+      </c>
       <c r="F26" s="4">
         <v>0.56145869640989898</v>
       </c>
@@ -1914,19 +1959,19 @@
       </c>
       <c r="K26" s="6">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="L26" s="6">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="M26" s="6">
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
-      <c r="N26" s="6" t="e">
-        <f t="shared" si="2"/>
-        <v>#N/A</v>
+      <c r="N26" s="6">
+        <f t="shared" si="2"/>
+        <v>5</v>
       </c>
       <c r="O26" s="6">
         <f t="shared" si="3"/>
@@ -1958,7 +2003,9 @@
       <c r="D27" s="4">
         <v>0.64925932380620399</v>
       </c>
-      <c r="E27" s="4"/>
+      <c r="E27" s="12">
+        <v>0.55415214360404297</v>
+      </c>
       <c r="F27" s="4">
         <v>0.55152056465667398</v>
       </c>
@@ -1975,19 +2022,19 @@
       </c>
       <c r="L27" s="6">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="M27" s="6">
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
-      <c r="N27" s="6" t="e">
-        <f t="shared" si="2"/>
-        <v>#N/A</v>
+      <c r="N27" s="6">
+        <f t="shared" si="2"/>
+        <v>5</v>
       </c>
       <c r="O27" s="6">
         <f t="shared" si="3"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="P27" s="6" t="e">
         <f t="shared" si="4"/>
@@ -2015,7 +2062,9 @@
       <c r="D28" s="4">
         <v>0.642079121645172</v>
       </c>
-      <c r="E28" s="4"/>
+      <c r="E28" s="12">
+        <v>0.55416085744161703</v>
+      </c>
       <c r="F28" s="4">
         <v>0.55883147438131697</v>
       </c>
@@ -2032,15 +2081,15 @@
       </c>
       <c r="L28" s="6">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="M28" s="6">
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
-      <c r="N28" s="6" t="e">
-        <f t="shared" si="2"/>
-        <v>#N/A</v>
+      <c r="N28" s="6">
+        <f t="shared" si="2"/>
+        <v>6</v>
       </c>
       <c r="O28" s="6">
         <f t="shared" si="3"/>
@@ -2072,7 +2121,9 @@
       <c r="D29" s="4">
         <v>0.63409288950853904</v>
       </c>
-      <c r="E29" s="4"/>
+      <c r="E29" s="12">
+        <v>0.55407807598466297</v>
+      </c>
       <c r="F29" s="4">
         <v>0.55084524224468401</v>
       </c>
@@ -2085,23 +2136,23 @@
       </c>
       <c r="K29" s="6">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="L29" s="6">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="M29" s="6">
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
-      <c r="N29" s="6" t="e">
-        <f t="shared" si="2"/>
-        <v>#N/A</v>
+      <c r="N29" s="6">
+        <f t="shared" si="2"/>
+        <v>4</v>
       </c>
       <c r="O29" s="6">
         <f t="shared" si="3"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="P29" s="6" t="e">
         <f t="shared" si="4"/>
@@ -2129,7 +2180,9 @@
       <c r="D30" s="4">
         <v>0.63668089926803695</v>
       </c>
-      <c r="E30" s="4"/>
+      <c r="E30" s="12">
+        <v>0.55418699895433898</v>
+      </c>
       <c r="F30" s="4">
         <v>0.56006448239804796</v>
       </c>
@@ -2142,19 +2195,19 @@
       </c>
       <c r="K30" s="6">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="L30" s="6">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="M30" s="6">
         <f t="shared" si="7"/>
         <v>2</v>
       </c>
-      <c r="N30" s="6" t="e">
-        <f t="shared" si="2"/>
-        <v>#N/A</v>
+      <c r="N30" s="6">
+        <f t="shared" si="2"/>
+        <v>5</v>
       </c>
       <c r="O30" s="6">
         <f t="shared" si="3"/>
@@ -2186,7 +2239,9 @@
       <c r="D31" s="4">
         <v>0.63146131056117105</v>
       </c>
-      <c r="E31" s="4"/>
+      <c r="E31" s="12">
+        <v>0.55410857441617201</v>
+      </c>
       <c r="F31" s="4">
         <v>0.54959044963401804</v>
       </c>
@@ -2203,19 +2258,19 @@
       </c>
       <c r="L31" s="6">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="M31" s="6">
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
-      <c r="N31" s="6" t="e">
-        <f t="shared" si="2"/>
-        <v>#N/A</v>
+      <c r="N31" s="6">
+        <f t="shared" si="2"/>
+        <v>5</v>
       </c>
       <c r="O31" s="6">
         <f t="shared" si="3"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="P31" s="6" t="e">
         <f t="shared" si="4"/>
@@ -2243,7 +2298,9 @@
       <c r="D32" s="4">
         <v>0.64663210177762198</v>
       </c>
-      <c r="E32" s="4"/>
+      <c r="E32" s="12">
+        <v>0.55413907284768205</v>
+      </c>
       <c r="F32" s="4">
         <v>0.55877919135587295</v>
       </c>
@@ -2256,7 +2313,7 @@
       </c>
       <c r="K32" s="6">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="L32" s="6">
         <f t="shared" si="1"/>
@@ -2266,9 +2323,9 @@
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
-      <c r="N32" s="6" t="e">
-        <f t="shared" si="2"/>
-        <v>#N/A</v>
+      <c r="N32" s="6">
+        <f t="shared" si="2"/>
+        <v>6</v>
       </c>
       <c r="O32" s="6">
         <f t="shared" si="3"/>
@@ -2300,7 +2357,9 @@
       <c r="D33" s="4">
         <v>0.64402666434297595</v>
       </c>
-      <c r="E33" s="4"/>
+      <c r="E33" s="12">
+        <v>0.55414778668525599</v>
+      </c>
       <c r="F33" s="4">
         <v>0.55614761240850397</v>
       </c>
@@ -2313,19 +2372,19 @@
       </c>
       <c r="K33" s="6">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="L33" s="6">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="M33" s="6">
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
-      <c r="N33" s="6" t="e">
-        <f t="shared" si="2"/>
-        <v>#N/A</v>
+      <c r="N33" s="6">
+        <f t="shared" si="2"/>
+        <v>5</v>
       </c>
       <c r="O33" s="6">
         <f t="shared" si="3"/>
@@ -2357,7 +2416,9 @@
       <c r="D34" s="4">
         <v>0.64204862321366296</v>
       </c>
-      <c r="E34" s="4"/>
+      <c r="E34" s="12">
+        <v>0.55415214360404297</v>
+      </c>
       <c r="F34" s="4">
         <v>0.54946409898919402</v>
       </c>
@@ -2370,23 +2431,23 @@
       </c>
       <c r="K34" s="6">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="L34" s="6">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="M34" s="6">
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
-      <c r="N34" s="6" t="e">
-        <f t="shared" si="2"/>
-        <v>#N/A</v>
+      <c r="N34" s="6">
+        <f t="shared" si="2"/>
+        <v>4</v>
       </c>
       <c r="O34" s="6">
         <f t="shared" si="3"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="P34" s="6" t="e">
         <f t="shared" si="4"/>
@@ -2414,7 +2475,9 @@
       <c r="D35" s="4">
         <v>0.64669745555942804</v>
       </c>
-      <c r="E35" s="4"/>
+      <c r="E35" s="12">
+        <v>0.55414342976646902</v>
+      </c>
       <c r="F35" s="4">
         <v>0.55614325548971699</v>
       </c>
@@ -2427,19 +2490,19 @@
       </c>
       <c r="K35" s="6">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="L35" s="6">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="M35" s="6">
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
-      <c r="N35" s="6" t="e">
-        <f t="shared" si="2"/>
-        <v>#N/A</v>
+      <c r="N35" s="6">
+        <f t="shared" si="2"/>
+        <v>5</v>
       </c>
       <c r="O35" s="6">
         <f t="shared" si="3"/>
@@ -2474,18 +2537,15 @@
         <f t="shared" si="8"/>
         <v>0.64031616707331196</v>
       </c>
-      <c r="E36" s="8" t="e">
+      <c r="E36" s="8">
         <f t="shared" si="8"/>
-        <v>#DIV/0!</v>
+        <v>0.55415867898222337</v>
       </c>
       <c r="F36" s="8">
         <f t="shared" si="8"/>
         <v>0.55740269548042221</v>
       </c>
-      <c r="G36" s="8" t="e">
-        <f t="shared" si="8"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="G36" s="8"/>
       <c r="H36" s="8">
         <f t="shared" si="8"/>
         <v>0.62756883931683483</v>
@@ -2496,23 +2556,23 @@
       </c>
       <c r="K36" s="9">
         <f t="shared" ref="K36:R36" si="9">AVERAGE(K6:K35)</f>
-        <v>5</v>
+        <v>5.7666666666666666</v>
       </c>
       <c r="L36" s="9">
         <f t="shared" si="9"/>
-        <v>5.7333333333333334</v>
+        <v>6.7</v>
       </c>
       <c r="M36" s="9">
         <f t="shared" si="9"/>
         <v>1.0666666666666667</v>
       </c>
-      <c r="N36" s="9" t="e">
+      <c r="N36" s="9">
         <f t="shared" si="9"/>
-        <v>#N/A</v>
+        <v>4.9666666666666668</v>
       </c>
       <c r="O36" s="9">
         <f t="shared" si="9"/>
-        <v>4.2666666666666666</v>
+        <v>4.5666666666666664</v>
       </c>
       <c r="P36" s="9" t="e">
         <f t="shared" si="9"/>
@@ -2536,22 +2596,22 @@
         <v>36</v>
       </c>
       <c r="D37" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="E37" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="E37" s="10" t="s">
+      <c r="F37" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="F37" s="10" t="s">
+      <c r="G37" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="G37" s="10" t="s">
-        <v>39</v>
-      </c>
       <c r="H37" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="I37" s="10" t="s">
         <v>41</v>
-      </c>
-      <c r="I37" s="10" t="s">
-        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>